<commit_message>
planilha controle de servicos atualizada
</commit_message>
<xml_diff>
--- a/Controle de servicços.xlsx
+++ b/Controle de servicços.xlsx
@@ -54,9 +54,6 @@
     <t>Nicolas</t>
   </si>
   <si>
-    <t>tela cad. Cidade</t>
-  </si>
-  <si>
     <t>Pedro</t>
   </si>
   <si>
@@ -143,6 +140,9 @@
       </rPr>
       <t>lider</t>
     </r>
+  </si>
+  <si>
+    <t>tela cidade</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -578,11 +578,11 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -593,11 +593,11 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -608,11 +608,11 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -625,11 +625,11 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -639,10 +639,12 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -657,7 +659,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -670,12 +672,12 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="5"/>
@@ -683,42 +685,40 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -726,15 +726,15 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -744,10 +744,10 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -757,10 +757,10 @@
     </row>
     <row r="16" spans="1:7" ht="15.75">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="1"/>

</xml_diff>

<commit_message>
Tela de Cadastro Referência Comercial
by: Pedro Enju
</commit_message>
<xml_diff>
--- a/Controle de servicços.xlsx
+++ b/Controle de servicços.xlsx
@@ -24,6 +24,9 @@
     <t>Nome:</t>
   </si>
   <si>
+    <t>Serviço:</t>
+  </si>
+  <si>
     <t>Alisson</t>
   </si>
   <si>
@@ -49,6 +52,9 @@
   </si>
   <si>
     <t>Nicolas</t>
+  </si>
+  <si>
+    <t>tela cad. Cidade</t>
   </si>
   <si>
     <t>Pedro</t>
@@ -137,12 +143,6 @@
       </rPr>
       <t>lider</t>
     </r>
-  </si>
-  <si>
-    <t>tela cidade</t>
-  </si>
-  <si>
-    <t>Serviço atuais:</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -573,98 +573,96 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="5"/>
@@ -672,12 +670,12 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="5"/>
@@ -685,40 +683,42 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -726,15 +726,15 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -744,10 +744,10 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -757,10 +757,10 @@
     </row>
     <row r="16" spans="1:7" ht="15.75">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="1"/>

</xml_diff>